<commit_message>
reision plan proyecto 1366
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1342 - RNCNOM, Moisés Meneses_OC/lineabase/Plan_de_proyecto.xlsx
+++ b/Proyectos/2015/11/P1342 - RNCNOM, Moisés Meneses_OC/lineabase/Plan_de_proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="158">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -651,9 +651,6 @@
     <t>Son equipos y sistemas con las adecuaciones necesarias desde nuestro ingreso a laborar</t>
   </si>
   <si>
-    <t xml:space="preserve">Falla de servicio electrico </t>
-  </si>
-  <si>
     <t>Home work</t>
   </si>
   <si>
@@ -661,9 +658,6 @@
   </si>
   <si>
     <t>Cerrado</t>
-  </si>
-  <si>
-    <t>Falla de servicio de internet</t>
   </si>
   <si>
     <t>Tener contrato con varias compañias de internet</t>
@@ -703,6 +697,15 @@
   </si>
   <si>
     <t>Se encuentran establecidos en las póliticas de la empresa</t>
+  </si>
+  <si>
+    <t>Ing. Ricardo González Novela</t>
+  </si>
+  <si>
+    <t>Falla de servicio eléctrico que evita la conexión de los dispositivos electrónicos</t>
+  </si>
+  <si>
+    <t>Falla de servicio de internet que impida la recepción y envío del certificado</t>
   </si>
 </sst>
 </file>
@@ -1544,15 +1547,15 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2590,7 +2593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
@@ -4824,10 +4827,10 @@
       <c r="D5"/>
     </row>
     <row r="6" spans="1:1023" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="126" t="s">
-        <v>155</v>
+      <c r="A6" s="129" t="s">
+        <v>153</v>
       </c>
-      <c r="B6" s="126"/>
+      <c r="B6" s="129"/>
       <c r="C6"/>
       <c r="D6"/>
     </row>
@@ -4840,10 +4843,10 @@
       <c r="D7"/>
     </row>
     <row r="8" spans="1:1023" ht="146.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="126" t="s">
-        <v>156</v>
+      <c r="A8" s="129" t="s">
+        <v>154</v>
       </c>
-      <c r="B8" s="126"/>
+      <c r="B8" s="129"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
@@ -4998,10 +5001,10 @@
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:4" ht="53.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="128" t="s">
+      <c r="A26" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="128"/>
+      <c r="B26" s="127"/>
       <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5011,10 +5014,10 @@
       <c r="B27" s="124"/>
     </row>
     <row r="28" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="127" t="s">
+      <c r="A28" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="128"/>
+      <c r="B28" s="127"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="124" t="s">
@@ -5023,13 +5026,18 @@
       <c r="B29" s="124"/>
     </row>
     <row r="30" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="129" t="s">
+      <c r="A30" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="129"/>
+      <c r="B30" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
@@ -5039,11 +5047,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A28" r:id="rId1"/>
@@ -24957,36 +24960,36 @@
     </row>
     <row r="6" spans="1:1023" s="38" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>115</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1023" s="38" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>111</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:1023" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -25256,8 +25259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:K6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26434,7 +26437,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="C5" s="59">
         <v>5</v>
@@ -26450,16 +26453,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="60" t="s">
-        <v>141</v>
-      </c>
       <c r="I5" s="62" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="J5" s="63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K5" s="64" t="s">
         <v>127</v>
@@ -27483,7 +27486,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C6" s="59">
         <v>5</v>
@@ -27499,16 +27502,16 @@
         <v>4</v>
       </c>
       <c r="G6" s="60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H6" s="60" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I6" s="62" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="J6" s="63" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K6" s="64" t="s">
         <v>127</v>

</xml_diff>